<commit_message>
Amend Cheque card status _Anandh
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSM_Master/TestData/CSMparamTestData.xlsx
+++ b/AzentioAutomationFramework_CSM_Master/TestData/CSMparamTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CSMParam_GeneralLedgerTestData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -460,6 +460,81 @@
   <si>
     <t>Update_data_set_id_1</t>
   </si>
+  <si>
+    <t>TRS</t>
+  </si>
+  <si>
+    <t>TRS_150_01</t>
+  </si>
+  <si>
+    <t>DS01_TRS_150_01</t>
+  </si>
+  <si>
+    <t>DS01_TRS_150</t>
+  </si>
+  <si>
+    <t>DS01_TRS_155</t>
+  </si>
+  <si>
+    <t>DS01_TRS_154</t>
+  </si>
+  <si>
+    <t>DS01_TRS_153</t>
+  </si>
+  <si>
+    <t>DS01_TRS_152</t>
+  </si>
+  <si>
+    <t>DS01_TRS_151</t>
+  </si>
+  <si>
+    <t>Update_data_set_id_2</t>
+  </si>
+  <si>
+    <t>Update_data_set_id_3</t>
+  </si>
+  <si>
+    <t>Update_data_set_id_4</t>
+  </si>
+  <si>
+    <t>Update_data_set_id_5</t>
+  </si>
+  <si>
+    <t>Update_data_set_id_6</t>
+  </si>
+  <si>
+    <t>AND OR</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>User Level</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>TRS_152_01</t>
+  </si>
+  <si>
+    <t>DS01_TRS_152_01</t>
+  </si>
+  <si>
+    <t>Dormant account dropdown</t>
+  </si>
+  <si>
+    <t>Proceed on Dormant A/C and view Signature</t>
+  </si>
+  <si>
+    <t>ANANDHTA</t>
+  </si>
 </sst>
 </file>
 
@@ -468,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -527,6 +602,13 @@
       <color rgb="FF111111"/>
       <name val="Consolas"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -675,7 +757,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -706,6 +788,8 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="3" fillId="10" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="5"/>
@@ -1023,7 +1107,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1039,14 +1123,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="33.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="32.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="27.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="33.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="22.85546875" collapsed="true"/>
-    <col min="8" max="16384" style="3" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="33.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="11" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1178,14 +1262,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="35.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="35.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="36.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="38.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="36.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="31.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="26.5703125" collapsed="true"/>
-    <col min="8" max="16384" style="3" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="35.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="11" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1270,30 +1354,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="34.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="35.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="3" width="33.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="37.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="38.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="49.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="21.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="16.28515625" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" style="3" width="20.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="3" width="28.140625" collapsed="true"/>
-    <col min="15" max="16384" style="3" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="34" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="38" style="3" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="28.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" style="3" collapsed="1"/>
+    <col min="17" max="17" width="11" style="3"/>
+    <col min="18" max="16384" width="11" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1328,16 +1417,19 @@
         <v>96</v>
       </c>
       <c r="L1" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -1364,8 +1456,9 @@
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="26"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1392,8 +1485,9 @@
       <c r="L3" s="26"/>
       <c r="M3" s="26"/>
       <c r="N3" s="26"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="26"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1418,8 +1512,9 @@
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="26"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="26"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1444,8 +1539,9 @@
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="26"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="26"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -1470,8 +1566,9 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="26"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="26"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -1496,8 +1593,9 @@
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="26"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="17" t="s">
         <v>80</v>
       </c>
@@ -1521,13 +1619,14 @@
         <v>100</v>
       </c>
       <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="26" t="s">
+      <c r="L8" s="26"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="26"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" s="26"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="20" t="s">
         <v>81</v>
       </c>
@@ -1551,13 +1650,14 @@
         <v>100</v>
       </c>
       <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="26" t="s">
+      <c r="L9" s="26"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="N9" s="26"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="26"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="17" t="s">
         <v>82</v>
       </c>
@@ -1581,15 +1681,16 @@
       <c r="K10" s="21">
         <v>100</v>
       </c>
-      <c r="L10" s="21"/>
-      <c r="M10" s="26" t="s">
+      <c r="L10" s="26"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="O10" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="20" t="s">
         <v>83</v>
       </c>
@@ -1613,13 +1714,14 @@
       <c r="K11" s="21">
         <v>100</v>
       </c>
-      <c r="L11" s="21"/>
-      <c r="M11" s="26" t="s">
+      <c r="L11" s="26"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="N11" s="26"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="26"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="17" t="s">
         <v>84</v>
       </c>
@@ -1643,13 +1745,14 @@
       <c r="K12" s="21">
         <v>100</v>
       </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="26" t="s">
+      <c r="L12" s="26"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="N12" s="26"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" s="26"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="20" t="s">
         <v>85</v>
       </c>
@@ -1673,13 +1776,14 @@
       <c r="K13" s="21">
         <v>100</v>
       </c>
-      <c r="L13" s="21"/>
-      <c r="M13" s="26" t="s">
+      <c r="L13" s="26"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="N13" s="26"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13" s="26"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="17" t="s">
         <v>86</v>
       </c>
@@ -1705,43 +1809,70 @@
         <v>300</v>
       </c>
       <c r="K14" s="21"/>
-      <c r="L14" s="21">
+      <c r="L14" s="26"/>
+      <c r="M14" s="21">
         <v>100</v>
       </c>
-      <c r="M14" s="26" t="s">
+      <c r="N14" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="N14" s="26"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="20" t="s">
-        <v>113</v>
+      <c r="O14" s="26"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="26"/>
-      <c r="I15" s="21">
-        <v>502</v>
-      </c>
+      <c r="I15" s="21"/>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="26" t="s">
+      <c r="L15" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="M15" s="21"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="21">
+        <v>502</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="N15" s="26"/>
+      <c r="O16" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="1.9306999999999999" bottom="1.9306999999999999" header="1.7338" footer="1.7338"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1755,18 +1886,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="31.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="35.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="32.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="42.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="36.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="32.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="29.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="37.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="28.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="3" width="13.5234375" collapsed="true"/>
-    <col min="12" max="16384" style="3" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="31.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="11" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1847,25 +1978,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="12" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:16" ht="15">
       <c r="A1" s="12" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -1882,11 +2015,38 @@
       <c r="F1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="29" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15">
+      <c r="L1" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15">
       <c r="A2" s="14" t="s">
         <v>66</v>
       </c>
@@ -1900,8 +2060,17 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-    </row>
-    <row r="3" spans="1:7" ht="15">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+    </row>
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" s="14" t="s">
         <v>68</v>
       </c>
@@ -1915,8 +2084,17 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" ht="15">
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+    </row>
+    <row r="4" spans="1:16" ht="15">
       <c r="A4" s="14" t="s">
         <v>69</v>
       </c>
@@ -1930,8 +2108,17 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" ht="15">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+    </row>
+    <row r="5" spans="1:16" ht="15">
       <c r="A5" s="14" t="s">
         <v>76</v>
       </c>
@@ -1945,8 +2132,17 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" ht="15">
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+    </row>
+    <row r="6" spans="1:16" ht="15">
       <c r="A6" s="14" t="s">
         <v>71</v>
       </c>
@@ -1960,8 +2156,17 @@
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="1:7" ht="15">
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:16" ht="15">
       <c r="A7" s="14" t="s">
         <v>72</v>
       </c>
@@ -1975,8 +2180,17 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" ht="15">
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" ht="15">
       <c r="A8" s="14" t="s">
         <v>74</v>
       </c>
@@ -1990,8 +2204,17 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:7" ht="13.5">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+    </row>
+    <row r="9" spans="1:16" ht="13.5">
       <c r="A9" s="20" t="s">
         <v>110</v>
       </c>
@@ -2005,23 +2228,87 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:7" ht="13.5">
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="1:16" ht="13.5">
       <c r="A10" s="20" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C10" s="21">
-        <v>502</v>
+        <v>977</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="19">
+        <v>1</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10" s="19">
+        <v>3</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="13.5">
+      <c r="A11" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="21">
+        <v>502</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19" t="s">
         <v>115</v>
       </c>
+      <c r="L11" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.0831" bottom="1.0831" header="0.88580000000000003" footer="0.88580000000000003"/>

</xml_diff>

<commit_message>
Chequebook Request code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSM_Master/TestData/CSMparamTestData.xlsx
+++ b/AzentioAutomationFramework_CSM_Master/TestData/CSMparamTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="CSMParam_GeneralLedgerTestData" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="ChargeCodeTestData" sheetId="6" r:id="rId6"/>
     <sheet name="Cheques_ChequeBookTestData" sheetId="7" r:id="rId7"/>
     <sheet name="CSMParam_ControlRecordsTestData" sheetId="8" r:id="rId8"/>
+    <sheet name="CSMParam_PriorityTestData" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="217">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -741,6 +742,27 @@
   </si>
   <si>
     <t>Branch</t>
+  </si>
+  <si>
+    <t>priority_code</t>
+  </si>
+  <si>
+    <t>waive_percentage</t>
+  </si>
+  <si>
+    <t>WP_CW_003_01</t>
+  </si>
+  <si>
+    <t>DS01_WP_CW_003_01</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
+    <t>update_dataset_id</t>
+  </si>
+  <si>
+    <t>DS01_WP_CW_003_02</t>
   </si>
 </sst>
 </file>
@@ -983,7 +1005,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1030,6 +1052,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="5"/>
@@ -3081,8 +3104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3128,4 +3151,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="38">
+        <v>1</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>